<commit_message>
Log reg model, added data and visualisation.
</commit_message>
<xml_diff>
--- a/output/log_reg_performance_data.xlsx
+++ b/output/log_reg_performance_data.xlsx
@@ -513,16 +513,16 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>10.30201654434204</v>
+        <v>10.83716549873352</v>
       </c>
       <c r="H2" t="n">
-        <v>45.1251350402832</v>
+        <v>62.82888569831848</v>
       </c>
       <c r="I2" t="n">
-        <v>3.271335458755493</v>
+        <v>3.744938850402832</v>
       </c>
       <c r="J2" t="n">
-        <v>59.00518460273743</v>
+        <v>77.67947835922241</v>
       </c>
       <c r="K2" t="n">
         <v>0.4809533943392211</v>
@@ -556,16 +556,16 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>10.08247952461243</v>
+        <v>9.58975796699524</v>
       </c>
       <c r="H3" t="n">
-        <v>29.31397500038147</v>
+        <v>28.7363639831543</v>
       </c>
       <c r="I3" t="n">
-        <v>3.010626316070557</v>
+        <v>2.95425181388855</v>
       </c>
       <c r="J3" t="n">
-        <v>42.59211258888244</v>
+        <v>41.57203869819641</v>
       </c>
       <c r="K3" t="n">
         <v>0.500373253705876</v>
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>13.1613242149353</v>
+        <v>13.54277448654175</v>
       </c>
       <c r="H4" t="n">
-        <v>43.89672431945801</v>
+        <v>46.2468533039093</v>
       </c>
       <c r="I4" t="n">
-        <v>4.674155282974243</v>
+        <v>4.371213436126709</v>
       </c>
       <c r="J4" t="n">
-        <v>61.99706950187683</v>
+        <v>64.38922328948975</v>
       </c>
       <c r="K4" t="n">
         <v>0.5263130252100841</v>
@@ -642,16 +642,16 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>19.90131826400757</v>
+        <v>29.63773217201233</v>
       </c>
       <c r="H5" t="n">
-        <v>180.3843579292297</v>
+        <v>232.3113450527191</v>
       </c>
       <c r="I5" t="n">
-        <v>13.88722267150879</v>
+        <v>24.56981449127197</v>
       </c>
       <c r="J5" t="n">
-        <v>214.5701570034027</v>
+        <v>286.7209562778473</v>
       </c>
       <c r="K5" t="n">
         <v>0.5394881587413604</v>
@@ -685,16 +685,16 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>88.46384267807007</v>
+        <v>104.0061954975128</v>
       </c>
       <c r="H6" t="n">
-        <v>481.2293424129486</v>
+        <v>618.1843870639801</v>
       </c>
       <c r="I6" t="n">
-        <v>28.38968296051025</v>
+        <v>84.07183785438538</v>
       </c>
       <c r="J6" t="n">
-        <v>598.3759604454041</v>
+        <v>806.6028195858001</v>
       </c>
       <c r="K6" t="n">
         <v>0.5502707183751716</v>

</xml_diff>